<commit_message>
Finished with small modifications needed
</commit_message>
<xml_diff>
--- a/schedule/scheduleData.xlsx
+++ b/schedule/scheduleData.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -427,17 +427,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="22.42578125" customWidth="1" min="1" max="1"/>
-    <col width="44" customWidth="1" min="2" max="2"/>
-    <col width="12.7109375" customWidth="1" min="3" max="4"/>
+    <col width="29.7109375" customWidth="1" min="1" max="1"/>
+    <col width="23.7109375" customWidth="1" min="2" max="2"/>
+    <col width="21.7109375" customWidth="1" min="3" max="3"/>
+    <col width="12.7109375" customWidth="1" min="4" max="4"/>
     <col width="11.85546875" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="12.42578125" customWidth="1" min="7" max="7"/>
@@ -447,97 +448,111 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>New Value</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Wednessday</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Time/Date</t>
+          <t>Sat Dec 20 11:45:56 2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Another Value</t>
+          <t>Basketball</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sat Dec 20 11:46:05 2025</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Voleyball</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="n">
-        <v>4</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sat Dec 20 11:46:11 2025</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Football</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sat Dec 20 11:46:14 2025</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sat Dec 20 11:46:26 2025</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Note writing</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sat Dec 20 11:46:33 2025</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CSC311</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>March 1st, 2026</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CSC321</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Feb. 14th, 2026</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Life coaching</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished with small modifications required
</commit_message>
<xml_diff>
--- a/schedule/scheduleData.xlsx
+++ b/schedule/scheduleData.xlsx
@@ -427,13 +427,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="29.7109375" customWidth="1" min="1" max="1"/>
     <col width="23.7109375" customWidth="1" min="2" max="2"/>
@@ -486,72 +486,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sat Dec 20 11:46:11 2025</t>
+          <t>March 14th, 2025</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Football</t>
+          <t>Cooking food</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sat Dec 20 11:46:14 2025</t>
+          <t>March 30th, 2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>  </t>
+          <t>Get a new phone</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sat Dec 20 11:46:26 2025</t>
+          <t>Tomorrow</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Note writing</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Sat Dec 20 11:46:33 2025</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>CSC311</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>March 1st, 2026</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>CSC321</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Feb. 14th, 2026</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Life coaching</t>
+          <t>CSC333</t>
         </is>
       </c>
     </row>

</xml_diff>